<commit_message>
Non working CSV and bucket creation
</commit_message>
<xml_diff>
--- a/HI-BOB_Dispatcher/Data/EmpNumbers.xlsx
+++ b/HI-BOB_Dispatcher/Data/EmpNumbers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sapconet365-my.sharepoint.com/personal/luan_hietbrink_sapconet_co_za/Documents/Documents/GitHub/HI-BOB/HI-BOB_Dispatcher/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sapconet365-my.sharepoint.com/personal/hanu_engelbrecht_sapconet_co_za/Documents/Documents/EPI-USE AUS/HI-BOB/HI-BOB_Dispatcher/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="11_F25DC773A252ABDACC10481E49585EE85BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C242B059-7B73-46D4-85D5-D13E643B2715}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_F25DC773A252ABDACC10481E49585EE85BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26EDBC0F-D275-422B-9DEB-2C96B57AD864}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -89,10 +89,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -358,1020 +354,3020 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A201"/>
+  <dimension ref="A1:A601"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H202" sqref="H202"/>
+    <sheetView tabSelected="1" topLeftCell="A601" workbookViewId="0">
+      <selection activeCell="A197" sqref="A197:A601"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>122465</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>135416</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>168978</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>649875</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>165497</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>165498</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>165499</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>165500</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>165501</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>165502</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>165503</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>165504</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>165505</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>165506</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>165507</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>165508</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>165509</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>165510</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>165511</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>165512</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>165513</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>165514</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>165515</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>165516</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>165517</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>165518</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>165519</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>165520</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>165521</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>165522</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>165523</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>165524</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>165525</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>165526</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>165527</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>165528</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>165529</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>165530</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>165531</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>165532</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>165533</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>165534</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>165535</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>165536</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>165537</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>165538</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>165539</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>165540</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>165541</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>165542</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>165543</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>165544</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>165545</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>165546</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>165547</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>165548</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>165549</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>165550</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>165551</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>165552</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>165553</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>165554</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>165555</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>165556</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>165557</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>165558</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>165559</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>165560</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>165561</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>165562</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>165563</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>165564</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>165565</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>165566</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>165567</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>165568</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>165569</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>165570</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>165571</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>165572</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>165573</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>165574</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>165575</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>165576</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>165577</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>165578</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>165579</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>165580</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>165581</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>165582</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>165583</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>165584</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>165585</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>165586</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>165587</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>165588</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>165589</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>165590</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>165591</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>165592</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>165593</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>165594</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>165595</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>165596</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>165597</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>165598</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>165599</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>165600</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>165601</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>165602</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>165603</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>165604</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>165605</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>165606</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>165607</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>165608</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>165609</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>165610</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>165611</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>165612</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>165613</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>165614</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>165615</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>165616</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>165617</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>165618</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>165619</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>165620</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>165621</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>165622</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>165623</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>165624</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>165625</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>165626</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>165627</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>165628</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>165629</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>165630</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>165631</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>165632</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>165633</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>165634</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>165635</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>165636</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>165637</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>165638</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>165639</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>165640</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>165641</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>165642</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>165643</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>165644</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>165645</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>165646</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>165647</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>165648</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>165649</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>165650</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>165651</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>165652</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>165653</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>165654</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>165655</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>165656</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>165657</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>165658</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>165659</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>165660</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>165661</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>165662</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>165663</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>165664</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>165665</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>165666</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>165667</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>165668</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>165669</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>165670</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>165671</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>165672</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>165673</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>165674</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>165675</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>165676</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>165677</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>165678</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>165679</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>165680</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>165681</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>165682</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>165683</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>165684</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>165685</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>165686</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>165687</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>165688</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>165689</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>165690</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>165691</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>165692</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A202">
+        <v>165693</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A203">
+        <v>165694</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A204">
+        <v>165695</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A205">
+        <v>165696</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A206">
+        <v>165697</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A207">
+        <v>165698</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A208">
+        <v>165699</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A209">
+        <v>165700</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A210">
+        <v>165701</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A211">
+        <v>165702</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A212">
+        <v>165703</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A213">
+        <v>165704</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A214">
+        <v>165705</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A215">
+        <v>165706</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A216">
+        <v>165707</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A217">
+        <v>165708</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A218">
+        <v>165709</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A219">
+        <v>165710</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A220">
+        <v>165711</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A221">
+        <v>165712</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A222">
+        <v>165713</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A223">
+        <v>165714</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A224">
+        <v>165715</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A225">
+        <v>165716</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A226">
+        <v>165717</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A227">
+        <v>165718</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A228">
+        <v>165719</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A229">
+        <v>165720</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A230">
+        <v>165721</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A231">
+        <v>165722</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A232">
+        <v>165723</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A233">
+        <v>165724</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A234">
+        <v>165725</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A235">
+        <v>165726</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A236">
+        <v>165727</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A237">
+        <v>165728</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A238">
+        <v>165729</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A239">
+        <v>165730</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A240">
+        <v>165731</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A241">
+        <v>165732</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A242">
+        <v>165733</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A243">
+        <v>165734</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A244">
+        <v>165735</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A245">
+        <v>165736</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A246">
+        <v>165737</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A247">
+        <v>165738</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A248">
+        <v>165739</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A249">
+        <v>165740</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A250">
+        <v>165741</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A251">
+        <v>165742</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A252">
+        <v>165743</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A253">
+        <v>165744</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A254">
+        <v>165745</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A255">
+        <v>165746</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A256">
+        <v>165747</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A257">
+        <v>165748</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A258">
+        <v>165749</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A259">
+        <v>165750</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A260">
+        <v>165751</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A261">
+        <v>165752</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A262">
+        <v>165753</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A263">
+        <v>165754</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A264">
+        <v>165755</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A265">
+        <v>165756</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A266">
+        <v>165757</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A267">
+        <v>165758</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A268">
+        <v>165759</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A269">
+        <v>165760</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A270">
+        <v>165761</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A271">
+        <v>165762</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A272">
+        <v>165763</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A273">
+        <v>165764</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A274">
+        <v>165765</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A275">
+        <v>165766</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A276">
+        <v>165767</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A277">
+        <v>165768</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A278">
+        <v>165769</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A279">
+        <v>165770</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A280">
+        <v>165771</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A281">
+        <v>165772</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A282">
+        <v>165773</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A283">
+        <v>165774</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A284">
+        <v>165775</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A285">
+        <v>165776</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A286">
+        <v>165777</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A287">
+        <v>165778</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A288">
+        <v>165779</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A289">
+        <v>165780</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A290">
+        <v>165781</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A291">
+        <v>165782</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A292">
+        <v>165783</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A293">
+        <v>165784</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A294">
+        <v>165785</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A295">
+        <v>165786</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A296">
+        <v>165787</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A297">
+        <v>165788</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A298">
+        <v>165789</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A299">
+        <v>165790</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A300">
+        <v>165791</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A301">
+        <v>165792</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A302">
+        <v>165793</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A303">
+        <v>165794</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A304">
+        <v>165795</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A305">
+        <v>165796</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A306">
+        <v>165797</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A307">
+        <v>165798</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A308">
+        <v>165799</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A309">
+        <v>165800</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A310">
+        <v>165801</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A311">
+        <v>165802</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A312">
+        <v>165803</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A313">
+        <v>165804</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A314">
+        <v>165805</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A315">
+        <v>165806</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A316">
+        <v>165807</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A317">
+        <v>165808</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A318">
+        <v>165809</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A319">
+        <v>165810</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A320">
+        <v>165811</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A321">
+        <v>165812</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A322">
+        <v>165813</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A323">
+        <v>165814</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A324">
+        <v>165815</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A325">
+        <v>165816</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A326">
+        <v>165817</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A327">
+        <v>165818</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A328">
+        <v>165819</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A329">
+        <v>165820</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A330">
+        <v>165821</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A331">
+        <v>165822</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A332">
+        <v>165823</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A333">
+        <v>165824</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A334">
+        <v>165825</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A335">
+        <v>165826</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A336">
+        <v>165827</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A337">
+        <v>165828</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A338">
+        <v>165829</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A339">
+        <v>165830</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A340">
+        <v>165831</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A341">
+        <v>165832</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A342">
+        <v>165833</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A343">
+        <v>165834</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A344">
+        <v>165835</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A345">
+        <v>165836</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A346">
+        <v>165837</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A347">
+        <v>165838</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A348">
+        <v>165839</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A349">
+        <v>165840</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A350">
+        <v>165841</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A351">
+        <v>165842</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A352">
+        <v>165843</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A353">
+        <v>165844</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A354">
+        <v>165845</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A355">
+        <v>165846</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A356">
+        <v>165847</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A357">
+        <v>165848</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A358">
+        <v>165849</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A359">
+        <v>165850</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A360">
+        <v>165851</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A361">
+        <v>165852</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A362">
+        <v>165853</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A363">
+        <v>165854</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A364">
+        <v>165855</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A365">
+        <v>165856</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A366">
+        <v>165857</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A367">
+        <v>165858</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A368">
+        <v>165859</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A369">
+        <v>165860</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A370">
+        <v>165861</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A371">
+        <v>165862</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A372">
+        <v>165863</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A373">
+        <v>165864</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A374">
+        <v>165865</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A375">
+        <v>165866</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A376">
+        <v>165867</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A377">
+        <v>165868</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A378">
+        <v>165869</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A379">
+        <v>165870</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A380">
+        <v>165871</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A381">
+        <v>165872</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A382">
+        <v>165873</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A383">
+        <v>165874</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A384">
+        <v>165875</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A385">
+        <v>165876</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A386">
+        <v>165877</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A387">
+        <v>165878</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A388">
+        <v>165879</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A389">
+        <v>165880</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A390">
+        <v>165881</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A391">
+        <v>165882</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A392">
+        <v>165883</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A393">
+        <v>165884</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A394">
+        <v>165885</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A395">
+        <v>165886</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A396">
+        <v>165887</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A397">
+        <v>165888</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A398">
+        <v>165889</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A399">
+        <v>165890</v>
+      </c>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A400">
+        <v>165891</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A401">
+        <v>165892</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A402">
+        <v>165893</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A403">
+        <v>165894</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A404">
+        <v>165895</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A405">
+        <v>165896</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A406">
+        <v>165897</v>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A407">
+        <v>165898</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A408">
+        <v>165899</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A409">
+        <v>165900</v>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A410">
+        <v>165901</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A411">
+        <v>165902</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A412">
+        <v>165903</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A413">
+        <v>165904</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A414">
+        <v>165905</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A415">
+        <v>165906</v>
+      </c>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A416">
+        <v>165907</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A417">
+        <v>165908</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A418">
+        <v>165909</v>
+      </c>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A419">
+        <v>165910</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A420">
+        <v>165911</v>
+      </c>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A421">
+        <v>165912</v>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A422">
+        <v>165913</v>
+      </c>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A423">
+        <v>165914</v>
+      </c>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A424">
+        <v>165915</v>
+      </c>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A425">
+        <v>165916</v>
+      </c>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A426">
+        <v>165917</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A427">
+        <v>165918</v>
+      </c>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A428">
+        <v>165919</v>
+      </c>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A429">
+        <v>165920</v>
+      </c>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A430">
+        <v>165921</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A431">
+        <v>165922</v>
+      </c>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A432">
+        <v>165923</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A433">
+        <v>165924</v>
+      </c>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A434">
+        <v>165925</v>
+      </c>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A435">
+        <v>165926</v>
+      </c>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A436">
+        <v>165927</v>
+      </c>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A437">
+        <v>165928</v>
+      </c>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A438">
+        <v>165929</v>
+      </c>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A439">
+        <v>165930</v>
+      </c>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A440">
+        <v>165931</v>
+      </c>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A441">
+        <v>165932</v>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A442">
+        <v>165933</v>
+      </c>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A443">
+        <v>165934</v>
+      </c>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A444">
+        <v>165935</v>
+      </c>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A445">
+        <v>165936</v>
+      </c>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A446">
+        <v>165937</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A447">
+        <v>165938</v>
+      </c>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A448">
+        <v>165939</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A449">
+        <v>165940</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A450">
+        <v>165941</v>
+      </c>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A451">
+        <v>165942</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A452">
+        <v>165943</v>
+      </c>
+    </row>
+    <row r="453" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A453">
+        <v>165944</v>
+      </c>
+    </row>
+    <row r="454" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A454">
+        <v>165945</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A455">
+        <v>165946</v>
+      </c>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A456">
+        <v>165947</v>
+      </c>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A457">
+        <v>165948</v>
+      </c>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A458">
+        <v>165949</v>
+      </c>
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A459">
+        <v>165950</v>
+      </c>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A460">
+        <v>165951</v>
+      </c>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A461">
+        <v>165952</v>
+      </c>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A462">
+        <v>165953</v>
+      </c>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A463">
+        <v>165954</v>
+      </c>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A464">
+        <v>165955</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A465">
+        <v>165956</v>
+      </c>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A466">
+        <v>165957</v>
+      </c>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A467">
+        <v>165958</v>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A468">
+        <v>165959</v>
+      </c>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A469">
+        <v>165960</v>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A470">
+        <v>165961</v>
+      </c>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A471">
+        <v>165962</v>
+      </c>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A472">
+        <v>165963</v>
+      </c>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A473">
+        <v>165964</v>
+      </c>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A474">
+        <v>165965</v>
+      </c>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A475">
+        <v>165966</v>
+      </c>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A476">
+        <v>165967</v>
+      </c>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A477">
+        <v>165968</v>
+      </c>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A478">
+        <v>165969</v>
+      </c>
+    </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A479">
+        <v>165970</v>
+      </c>
+    </row>
+    <row r="480" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A480">
+        <v>165971</v>
+      </c>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A481">
+        <v>165972</v>
+      </c>
+    </row>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A482">
+        <v>165973</v>
+      </c>
+    </row>
+    <row r="483" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A483">
+        <v>165974</v>
+      </c>
+    </row>
+    <row r="484" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A484">
+        <v>165975</v>
+      </c>
+    </row>
+    <row r="485" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A485">
+        <v>165976</v>
+      </c>
+    </row>
+    <row r="486" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A486">
+        <v>165977</v>
+      </c>
+    </row>
+    <row r="487" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A487">
+        <v>165978</v>
+      </c>
+    </row>
+    <row r="488" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A488">
+        <v>165979</v>
+      </c>
+    </row>
+    <row r="489" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A489">
+        <v>165980</v>
+      </c>
+    </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A490">
+        <v>165981</v>
+      </c>
+    </row>
+    <row r="491" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A491">
+        <v>165982</v>
+      </c>
+    </row>
+    <row r="492" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A492">
+        <v>165983</v>
+      </c>
+    </row>
+    <row r="493" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A493">
+        <v>165984</v>
+      </c>
+    </row>
+    <row r="494" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A494">
+        <v>165985</v>
+      </c>
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A495">
+        <v>165986</v>
+      </c>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A496">
+        <v>165987</v>
+      </c>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A497">
+        <v>165988</v>
+      </c>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A498">
+        <v>165989</v>
+      </c>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A499">
+        <v>165990</v>
+      </c>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A500">
+        <v>165991</v>
+      </c>
+    </row>
+    <row r="501" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A501">
+        <v>165992</v>
+      </c>
+    </row>
+    <row r="502" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A502">
+        <v>165993</v>
+      </c>
+    </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A503">
+        <v>165994</v>
+      </c>
+    </row>
+    <row r="504" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A504">
+        <v>165995</v>
+      </c>
+    </row>
+    <row r="505" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A505">
+        <v>165996</v>
+      </c>
+    </row>
+    <row r="506" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A506">
+        <v>165997</v>
+      </c>
+    </row>
+    <row r="507" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A507">
+        <v>165998</v>
+      </c>
+    </row>
+    <row r="508" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A508">
+        <v>165999</v>
+      </c>
+    </row>
+    <row r="509" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A509">
+        <v>166000</v>
+      </c>
+    </row>
+    <row r="510" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A510">
+        <v>166001</v>
+      </c>
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A511">
+        <v>166002</v>
+      </c>
+    </row>
+    <row r="512" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A512">
+        <v>166003</v>
+      </c>
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A513">
+        <v>166004</v>
+      </c>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A514">
+        <v>166005</v>
+      </c>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A515">
+        <v>166006</v>
+      </c>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A516">
+        <v>166007</v>
+      </c>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A517">
+        <v>166008</v>
+      </c>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A518">
+        <v>166009</v>
+      </c>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A519">
+        <v>166010</v>
+      </c>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A520">
+        <v>166011</v>
+      </c>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A521">
+        <v>166012</v>
+      </c>
+    </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A522">
+        <v>166013</v>
+      </c>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A523">
+        <v>166014</v>
+      </c>
+    </row>
+    <row r="524" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A524">
+        <v>166015</v>
+      </c>
+    </row>
+    <row r="525" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A525">
+        <v>166016</v>
+      </c>
+    </row>
+    <row r="526" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A526">
+        <v>166017</v>
+      </c>
+    </row>
+    <row r="527" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A527">
+        <v>166018</v>
+      </c>
+    </row>
+    <row r="528" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A528">
+        <v>166019</v>
+      </c>
+    </row>
+    <row r="529" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A529">
+        <v>166020</v>
+      </c>
+    </row>
+    <row r="530" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A530">
+        <v>166021</v>
+      </c>
+    </row>
+    <row r="531" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A531">
+        <v>166022</v>
+      </c>
+    </row>
+    <row r="532" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A532">
+        <v>166023</v>
+      </c>
+    </row>
+    <row r="533" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A533">
+        <v>166024</v>
+      </c>
+    </row>
+    <row r="534" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A534">
+        <v>166025</v>
+      </c>
+    </row>
+    <row r="535" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A535">
+        <v>166026</v>
+      </c>
+    </row>
+    <row r="536" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A536">
+        <v>166027</v>
+      </c>
+    </row>
+    <row r="537" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A537">
+        <v>166028</v>
+      </c>
+    </row>
+    <row r="538" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A538">
+        <v>166029</v>
+      </c>
+    </row>
+    <row r="539" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A539">
+        <v>166030</v>
+      </c>
+    </row>
+    <row r="540" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A540">
+        <v>166031</v>
+      </c>
+    </row>
+    <row r="541" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A541">
+        <v>166032</v>
+      </c>
+    </row>
+    <row r="542" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A542">
+        <v>166033</v>
+      </c>
+    </row>
+    <row r="543" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A543">
+        <v>166034</v>
+      </c>
+    </row>
+    <row r="544" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A544">
+        <v>166035</v>
+      </c>
+    </row>
+    <row r="545" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A545">
+        <v>166036</v>
+      </c>
+    </row>
+    <row r="546" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A546">
+        <v>166037</v>
+      </c>
+    </row>
+    <row r="547" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A547">
+        <v>166038</v>
+      </c>
+    </row>
+    <row r="548" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A548">
+        <v>166039</v>
+      </c>
+    </row>
+    <row r="549" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A549">
+        <v>166040</v>
+      </c>
+    </row>
+    <row r="550" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A550">
+        <v>166041</v>
+      </c>
+    </row>
+    <row r="551" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A551">
+        <v>166042</v>
+      </c>
+    </row>
+    <row r="552" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A552">
+        <v>166043</v>
+      </c>
+    </row>
+    <row r="553" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A553">
+        <v>166044</v>
+      </c>
+    </row>
+    <row r="554" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A554">
+        <v>166045</v>
+      </c>
+    </row>
+    <row r="555" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A555">
+        <v>166046</v>
+      </c>
+    </row>
+    <row r="556" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A556">
+        <v>166047</v>
+      </c>
+    </row>
+    <row r="557" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A557">
+        <v>166048</v>
+      </c>
+    </row>
+    <row r="558" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A558">
+        <v>166049</v>
+      </c>
+    </row>
+    <row r="559" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A559">
+        <v>166050</v>
+      </c>
+    </row>
+    <row r="560" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A560">
+        <v>166051</v>
+      </c>
+    </row>
+    <row r="561" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A561">
+        <v>166052</v>
+      </c>
+    </row>
+    <row r="562" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A562">
+        <v>166053</v>
+      </c>
+    </row>
+    <row r="563" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A563">
+        <v>166054</v>
+      </c>
+    </row>
+    <row r="564" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A564">
+        <v>166055</v>
+      </c>
+    </row>
+    <row r="565" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A565">
+        <v>166056</v>
+      </c>
+    </row>
+    <row r="566" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A566">
+        <v>166057</v>
+      </c>
+    </row>
+    <row r="567" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A567">
+        <v>166058</v>
+      </c>
+    </row>
+    <row r="568" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A568">
+        <v>166059</v>
+      </c>
+    </row>
+    <row r="569" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A569">
+        <v>166060</v>
+      </c>
+    </row>
+    <row r="570" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A570">
+        <v>166061</v>
+      </c>
+    </row>
+    <row r="571" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A571">
+        <v>166062</v>
+      </c>
+    </row>
+    <row r="572" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A572">
+        <v>166063</v>
+      </c>
+    </row>
+    <row r="573" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A573">
+        <v>166064</v>
+      </c>
+    </row>
+    <row r="574" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A574">
+        <v>166065</v>
+      </c>
+    </row>
+    <row r="575" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A575">
+        <v>166066</v>
+      </c>
+    </row>
+    <row r="576" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A576">
+        <v>166067</v>
+      </c>
+    </row>
+    <row r="577" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A577">
+        <v>166068</v>
+      </c>
+    </row>
+    <row r="578" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A578">
+        <v>166069</v>
+      </c>
+    </row>
+    <row r="579" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A579">
+        <v>166070</v>
+      </c>
+    </row>
+    <row r="580" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A580">
+        <v>166071</v>
+      </c>
+    </row>
+    <row r="581" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A581">
+        <v>166072</v>
+      </c>
+    </row>
+    <row r="582" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A582">
+        <v>166073</v>
+      </c>
+    </row>
+    <row r="583" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A583">
+        <v>166074</v>
+      </c>
+    </row>
+    <row r="584" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A584">
+        <v>166075</v>
+      </c>
+    </row>
+    <row r="585" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A585">
+        <v>166076</v>
+      </c>
+    </row>
+    <row r="586" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A586">
+        <v>166077</v>
+      </c>
+    </row>
+    <row r="587" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A587">
+        <v>166078</v>
+      </c>
+    </row>
+    <row r="588" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A588">
+        <v>166079</v>
+      </c>
+    </row>
+    <row r="589" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A589">
+        <v>166080</v>
+      </c>
+    </row>
+    <row r="590" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A590">
+        <v>166081</v>
+      </c>
+    </row>
+    <row r="591" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A591">
+        <v>166082</v>
+      </c>
+    </row>
+    <row r="592" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A592">
+        <v>166083</v>
+      </c>
+    </row>
+    <row r="593" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A593">
+        <v>166084</v>
+      </c>
+    </row>
+    <row r="594" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A594">
+        <v>166085</v>
+      </c>
+    </row>
+    <row r="595" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A595">
+        <v>166086</v>
+      </c>
+    </row>
+    <row r="596" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A596">
+        <v>166087</v>
+      </c>
+    </row>
+    <row r="597" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A597">
+        <v>166088</v>
+      </c>
+    </row>
+    <row r="598" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A598">
+        <v>166089</v>
+      </c>
+    </row>
+    <row r="599" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A599">
+        <v>166090</v>
+      </c>
+    </row>
+    <row r="600" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A600">
+        <v>166091</v>
+      </c>
+    </row>
+    <row r="601" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A601">
+        <v>166092</v>
       </c>
     </row>
   </sheetData>

</xml_diff>